<commit_message>
add excel txt file read
</commit_message>
<xml_diff>
--- a/ExcelTemplate02.xlsx
+++ b/ExcelTemplate02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personel\Project\ISO.PDFSearchApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428107AD-B786-4D2B-9C73-7297C8FE086C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D874D-7F92-40B7-A301-DA36E1380D02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="1896" windowWidth="18708" windowHeight="8388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,7 +632,7 @@
     <col min="4" max="4" width="14.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="41.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="4.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="13" customWidth="1"/>
     <col min="8" max="8" width="4.5546875" style="13" customWidth="1"/>
     <col min="9" max="9" width="4.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.88671875" style="13" bestFit="1" customWidth="1"/>

</xml_diff>